<commit_message>
UPDATE technology portfolios for Norway
</commit_message>
<xml_diff>
--- a/inputs/ab.xlsx
+++ b/inputs/ab.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Documents\district_thermal_energy_systems_with_power_markets\source_code\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Documents\district_thermal_energy_systems_with_power_markets\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A88D80E-9F3A-4E97-B0CD-8A949F991186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{227A8A9A-F3F1-4E67-9897-A5643B72E593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-1965" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025" sheetId="1" r:id="rId1"/>
@@ -395,13 +395,13 @@
         <v>0.7</v>
       </c>
       <c r="B2">
-        <v>6.0525000000000002</v>
+        <v>8.5787499999999994</v>
       </c>
       <c r="C2">
-        <v>966532.6</v>
+        <v>878666</v>
       </c>
       <c r="D2">
-        <v>396000</v>
+        <v>360000</v>
       </c>
     </row>
   </sheetData>
@@ -436,15 +436,15 @@
         <v>0.7</v>
       </c>
       <c r="B2">
-        <v>6.0525000000000002</v>
+        <v>8.5787499999999994</v>
       </c>
       <c r="C2">
         <f>'2025'!C2*(1-0.25*0.2)</f>
-        <v>918205.97</v>
+        <v>834732.7</v>
       </c>
       <c r="D2">
         <f>'2025'!D2*(1-0.25*0.2)</f>
-        <v>376200</v>
+        <v>342000</v>
       </c>
     </row>
   </sheetData>
@@ -479,15 +479,15 @@
         <v>0.7</v>
       </c>
       <c r="B2">
-        <v>6.0525000000000002</v>
+        <v>8.5787499999999994</v>
       </c>
       <c r="C2">
         <f>'2025'!C2*(1-0.25*0.4)</f>
-        <v>869879.34</v>
+        <v>790799.4</v>
       </c>
       <c r="D2">
         <f>'2025'!D2*(1-0.25*0.4)</f>
-        <v>356400</v>
+        <v>324000</v>
       </c>
     </row>
   </sheetData>
@@ -522,15 +522,15 @@
         <v>0.7</v>
       </c>
       <c r="B2">
-        <v>6.0525000000000002</v>
+        <v>8.5787499999999994</v>
       </c>
       <c r="C2">
         <f>'2025'!C2*(1-0.25*0.6)</f>
-        <v>821552.71</v>
+        <v>746866.1</v>
       </c>
       <c r="D2">
         <f>'2025'!D2*(1-0.25*0.6)</f>
-        <v>336600</v>
+        <v>306000</v>
       </c>
     </row>
   </sheetData>
@@ -565,15 +565,15 @@
         <v>0.7</v>
       </c>
       <c r="B2">
-        <v>6.0525000000000002</v>
+        <v>8.5787499999999994</v>
       </c>
       <c r="C2">
         <f>'2025'!C2*(1-0.25*0.8)</f>
-        <v>773226.08000000007</v>
+        <v>702932.8</v>
       </c>
       <c r="D2">
         <f>'2025'!D2*(1-0.25*0.8)</f>
-        <v>316800</v>
+        <v>288000</v>
       </c>
     </row>
   </sheetData>
@@ -608,15 +608,15 @@
         <v>0.7</v>
       </c>
       <c r="B2">
-        <v>6.0525000000000002</v>
+        <v>8.5787499999999994</v>
       </c>
       <c r="C2">
         <f>'2025'!C2*(1-0.25*1)</f>
-        <v>724899.45</v>
+        <v>658999.5</v>
       </c>
       <c r="D2">
         <f>'2025'!D2*(1-0.25*1)</f>
-        <v>297000</v>
+        <v>270000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>